<commit_message>
Update supplier onboarding template with new data and formatting improvements
</commit_message>
<xml_diff>
--- a/src/assets/supplier_onboarding_template.xlsx
+++ b/src/assets/supplier_onboarding_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B78A3C-9AF9-4441-94D7-939EF41362E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60F4D20A-D430-4184-81A0-2EFA8B82CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Product Name</t>
   </si>
@@ -42,24 +42,39 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Supplier</t>
+    <t>Description</t>
   </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>Current Quantity</t>
-  </si>
-  <si>
-    <t>productStockLevel</t>
-  </si>
-  <si>
-    <t>Percentage Available</t>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>HS Code</t>
+  </si>
+  <si>
+    <t>Country of Origin</t>
   </si>
   <si>
     <t>Warehouse Location</t>
   </si>
   <si>
+    <t>Weight (ounces)</t>
+  </si>
+  <si>
+    <t>Height (inches)</t>
+  </si>
+  <si>
+    <t>Length (inches)</t>
+  </si>
+  <si>
+    <t>Width (inches)</t>
+  </si>
+  <si>
+    <t>Product Image Url</t>
+  </si>
+  <si>
     <t>Champagne Bottle</t>
   </si>
   <si>
@@ -69,13 +84,16 @@
     <t>Beverages</t>
   </si>
   <si>
-    <t>Luxury Liquor Co.</t>
-  </si>
-  <si>
-    <t>$120.00</t>
-  </si>
-  <si>
-    <t>Cellar-1</t>
+    <t>Sparkling wine (including champagne)</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Warehouse-1</t>
+  </si>
+  <si>
+    <t>https://tse3.mm.bing.net/th/id/OIP.caEYlp7WHARd2U7BAZ_hXAHaHa?rs=1&amp;pid=ImgDetMain&amp;o=7&amp;rm=3</t>
   </si>
   <si>
     <t>Marine First Aid Kit</t>
@@ -87,20 +105,24 @@
     <t>Safety Equipment</t>
   </si>
   <si>
-    <t>Marine Essentials Inc.</t>
-  </si>
-  <si>
-    <t>MedBay-2</t>
+    <t>First-aid boxes and kits</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>https://tse4.mm.bing.net/th/id/OIP.oxGPo9sN1XhhTWpt6jDuvgHaE8?rs=1&amp;pid=ImgDetMain&amp;o=7&amp;rm=3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +134,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,10 +186,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -160,8 +198,15 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,25 +509,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,66 +560,115 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>2204.1</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
+      <c r="M2">
+        <v>9</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E3" s="4">
         <v>150</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>20000</v>
       </c>
       <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.1</v>
+        <v>3006.5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
       </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>18</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{A4F491A0-77A1-463A-8318-6D4E62D3C9D1}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{99370A90-7CCF-4BFE-93DA-446F04A4F23E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>